<commit_message>
fix review code & checklist
</commit_message>
<xml_diff>
--- a/3.Js/react/tri/ER/checklist/Checklist_code_resetpassword.xlsx
+++ b/3.Js/react/tri/ER/checklist/Checklist_code_resetpassword.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\app\demo\training_web\3.Js\react\tri\ER\checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="2" r:id="rId1"/>
@@ -678,10 +678,10 @@
     <t>a). Các folder con nằm trong /container || /component || /views  sẽ đặt tên theo dạng PascalCase (viết hoa 2 chữ đầu tiên)</t>
   </si>
   <si>
-    <t>Project Code: Vue Checklist _ resetpassword</t>
+    <t>o</t>
   </si>
   <si>
-    <t>o</t>
+    <t>Project Code: Checklist _ resetpassword</t>
   </si>
 </sst>
 </file>
@@ -1998,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -2527,7 +2527,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -2539,7 +2539,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -2561,7 +2561,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="21"/>
@@ -2585,7 +2585,7 @@
         <v>51</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -2599,7 +2599,7 @@
       <c r="B26" s="27"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
@@ -2611,7 +2611,7 @@
       <c r="B27" s="27"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
@@ -2621,7 +2621,7 @@
         <v>54</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
@@ -2633,7 +2633,7 @@
         <v>55</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
@@ -2645,7 +2645,7 @@
         <v>56</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -2659,7 +2659,7 @@
       <c r="B31" s="27"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
@@ -2669,7 +2669,7 @@
         <v>58</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
@@ -2691,7 +2691,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
@@ -2703,7 +2703,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
@@ -2715,7 +2715,7 @@
         <v>84</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
@@ -2727,7 +2727,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
@@ -2739,7 +2739,7 @@
         <v>62</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
@@ -2751,7 +2751,7 @@
         <v>63</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
@@ -2763,7 +2763,7 @@
         <v>64</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
@@ -2775,7 +2775,7 @@
         <v>65</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
@@ -2797,7 +2797,7 @@
         <v>67</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
@@ -2809,7 +2809,7 @@
         <v>68</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21"/>
@@ -2821,7 +2821,7 @@
         <v>69</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
@@ -2833,7 +2833,7 @@
         <v>70</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
@@ -2845,7 +2845,7 @@
         <v>71</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -2857,7 +2857,7 @@
         <v>72</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -2869,7 +2869,7 @@
         <v>73</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
@@ -2881,7 +2881,7 @@
         <v>74</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
@@ -2893,7 +2893,7 @@
         <v>75</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
@@ -2905,7 +2905,7 @@
         <v>76</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
@@ -2917,7 +2917,7 @@
         <v>77</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -2931,7 +2931,7 @@
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E54" s="21"/>
       <c r="F54" s="22"/>

</xml_diff>